<commit_message>
Updated default jtot and SPC
</commit_message>
<xml_diff>
--- a/DataForTEA.xlsx
+++ b/DataForTEA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Experimental/LCA TEA for CO2R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="725" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FEF3CBE-AAA3-4FE5-962B-BBCE2FFBD4C4}"/>
+  <xr:revisionPtr revIDLastSave="731" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF698F68-0AF1-4892-B513-F8F0B5A4B78D}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -6031,15 +6031,15 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="25.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.88671875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>221</v>
       </c>
@@ -6073,7 +6073,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>146</v>
       </c>
@@ -6091,7 +6091,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>165</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>225</v>
       </c>
@@ -6130,7 +6130,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>148</v>
       </c>
@@ -6146,7 +6146,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>149</v>
       </c>
@@ -6162,7 +6162,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>150</v>
       </c>
@@ -6178,7 +6178,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>151</v>
       </c>
@@ -6194,7 +6194,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>145</v>
       </c>
@@ -6210,7 +6210,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>162</v>
       </c>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>169</v>
       </c>
@@ -6244,7 +6244,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>143</v>
       </c>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>152</v>
       </c>
@@ -6278,7 +6278,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>160</v>
       </c>
@@ -6294,7 +6294,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>147</v>
       </c>
@@ -6310,7 +6310,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>159</v>
       </c>
@@ -6326,7 +6326,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>157</v>
       </c>
@@ -6342,7 +6342,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>167</v>
       </c>
@@ -6358,7 +6358,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>158</v>
       </c>
@@ -6374,7 +6374,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>173</v>
       </c>
@@ -6389,7 +6389,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>178</v>
       </c>
@@ -6403,7 +6403,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>175</v>
       </c>
@@ -6419,7 +6419,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>170</v>
       </c>
@@ -6435,7 +6435,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>231</v>
       </c>
@@ -6451,7 +6451,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>168</v>
       </c>
@@ -6465,7 +6465,7 @@
       <c r="E26" s="24"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>166</v>
       </c>
@@ -6481,7 +6481,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>161</v>
       </c>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>144</v>
       </c>
@@ -6517,7 +6517,7 @@
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>142</v>
       </c>
@@ -6536,7 +6536,7 @@
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>163</v>
       </c>
@@ -6554,7 +6554,7 @@
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>164</v>
       </c>
@@ -6570,7 +6570,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>153</v>
       </c>
@@ -6586,7 +6586,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>154</v>
       </c>
@@ -6603,7 +6603,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>155</v>
       </c>
@@ -6620,7 +6620,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>156</v>
       </c>
@@ -6636,46 +6636,46 @@
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
     </row>
@@ -6705,30 +6705,30 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N6" sqref="N6"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="15.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.109375" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.88671875" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="57" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>78</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>99</v>
       </c>
@@ -6819,7 +6819,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>63</v>
       </c>
@@ -6861,10 +6861,10 @@
         <v>0.95</v>
       </c>
       <c r="N3" s="73">
-        <v>0.1138</v>
+        <v>0.1148</v>
       </c>
       <c r="O3" s="74">
-        <v>511.8</v>
+        <v>472.1</v>
       </c>
       <c r="P3" s="24" t="s">
         <v>20</v>
@@ -6873,7 +6873,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>83</v>
       </c>
@@ -6914,10 +6914,10 @@
         <v>0.7</v>
       </c>
       <c r="N4" s="73">
-        <v>2.6190000000000001E-2</v>
+        <v>2.6550000000000001E-2</v>
       </c>
       <c r="O4" s="74">
-        <v>475.2</v>
+        <v>435.9</v>
       </c>
       <c r="P4" s="24" t="s">
         <v>20</v>
@@ -6926,7 +6926,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>86</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>84</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>85</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>88</v>
       </c>
@@ -7094,7 +7094,7 @@
       <c r="P8" s="24"/>
       <c r="Q8" s="34"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>87</v>
       </c>
@@ -7129,7 +7129,7 @@
       <c r="P9" s="24"/>
       <c r="Q9" s="34"/>
     </row>
-    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>92</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>Jouny, Jiao I&amp;EC 2022</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>93</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>Jouny, Jiao I&amp;EC 2019 - but $0.6 Guerra 2023</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>94</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>Jouny, Jiao I&amp;EC 2021 - but $0.5 Guerra 2023</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>96</v>
       </c>
@@ -7293,7 +7293,7 @@
       <c r="P13" s="24"/>
       <c r="Q13" s="34"/>
     </row>
-    <row r="14" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>97</v>
       </c>
@@ -7331,7 +7331,7 @@
       <c r="P14" s="24"/>
       <c r="Q14" s="34"/>
     </row>
-    <row r="15" spans="1:17" s="32" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="32" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>24</v>
       </c>
@@ -7401,18 +7401,18 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="43" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="31.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="43" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="3"/>
+    <col min="6" max="6" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -7426,13 +7426,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="41"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>136</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>133</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
@@ -7500,7 +7500,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>49</v>
       </c>
@@ -7544,13 +7544,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="41"/>
       <c r="C10" s="47"/>
       <c r="D10" s="47"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="D11" s="47"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>26</v>
       </c>
@@ -7578,13 +7578,13 @@
       </c>
       <c r="D12" s="47"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="42"/>
       <c r="C13" s="47"/>
       <c r="D13" s="47"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>116</v>
       </c>
@@ -7622,15 +7622,15 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -7661,7 +7661,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>13865294.437769506</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -7763,7 +7763,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
         <v>62</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>66</v>
       </c>
@@ -7811,7 +7811,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D12" s="28">
         <v>30</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D13" s="27">
         <f>D12*K15</f>
         <v>7.0299214812573688E-2</v>
@@ -7847,7 +7847,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D14" s="28">
         <v>5</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>61</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>181</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>180</v>
       </c>
@@ -7907,7 +7907,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -7919,7 +7919,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>180</v>
       </c>
@@ -7935,7 +7935,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20">
         <f>B19*1000</f>
         <v>321.08784381927757</v>
@@ -7948,7 +7948,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -7974,15 +7974,15 @@
       <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="13.7109375" style="51"/>
-    <col min="9" max="15" width="13.7109375" style="52"/>
-    <col min="16" max="16" width="20.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="13.7109375" style="51"/>
+    <col min="1" max="8" width="13.6640625" style="51"/>
+    <col min="9" max="15" width="13.6640625" style="52"/>
+    <col min="16" max="16" width="20.5546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="13.6640625" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
         <v>198</v>
       </c>
@@ -7990,7 +7990,7 @@
       <c r="C1" s="57"/>
       <c r="D1" s="57"/>
     </row>
-    <row r="2" spans="1:27" s="52" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="52" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="67" t="s">
         <v>199</v>
       </c>
@@ -8000,7 +8000,7 @@
       <c r="E2" s="51"/>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
@@ -8017,7 +8017,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
         <v>6</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>13</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>2382.3538795879008</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -8119,7 +8119,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>204</v>
       </c>
@@ -8134,7 +8134,7 @@
       <c r="F9" s="51"/>
       <c r="L9" s="51"/>
     </row>
-    <row r="10" spans="1:27" s="52" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" s="52" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>205</v>
       </c>
@@ -8150,7 +8150,7 @@
       <c r="F10" s="51"/>
       <c r="L10" s="51"/>
     </row>
-    <row r="11" spans="1:27" s="52" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" s="52" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>200</v>
       </c>
@@ -8166,7 +8166,7 @@
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
     </row>
-    <row r="12" spans="1:27" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" s="52" customFormat="1" ht="29.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>201</v>
       </c>
@@ -8182,7 +8182,7 @@
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -8190,10 +8190,10 @@
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B14" s="52"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="76" t="s">
         <v>206</v>
       </c>
@@ -8214,7 +8214,7 @@
       <c r="O17" s="76"/>
       <c r="P17" s="76"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="75" t="s">
         <v>195</v>
       </c>
@@ -8244,7 +8244,7 @@
       <c r="O18" s="75"/>
       <c r="P18" s="75"/>
     </row>
-    <row r="19" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A19" s="55" t="s">
         <v>208</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="60">
         <v>-51.5244564886654</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>5.0730403065140095E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="60">
         <v>-89.797974315320403</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>6.5460850237780699E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="60">
         <v>-128.06720097650799</v>
       </c>
@@ -8460,7 +8460,7 @@
         <v>8.6704673566159185E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="60">
         <v>-166.34194485043901</v>
       </c>
@@ -8516,7 +8516,7 @@
         <v>1.1771856112818058E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="60">
         <v>-204.613623606179</v>
       </c>
@@ -8572,7 +8572,7 @@
         <v>1.6610145177220037E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="60">
         <v>-242.881624220091</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>2.2533996934247069E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="60">
         <v>-281.15268995219299</v>
       </c>
@@ -8684,7 +8684,7 @@
         <v>3.149742423062496E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="60">
         <v>-319.427433826124</v>
       </c>
@@ -8740,7 +8740,7 @@
         <v>4.8494015452431039E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="60">
         <v>-357.69420839275898</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>7.7219536858392002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="60">
         <v>-395.96343505394702</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>0.10626191485734104</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="60">
         <v>-434.23572683332497</v>
       </c>
@@ -8908,7 +8908,7 @@
         <v>-1.8498964897695203E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="60">
         <v>-472.50188837632197</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>-1.3483050770102256E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="60">
         <v>-510.774180155701</v>
       </c>
@@ -9007,7 +9007,7 @@
       <c r="O32" s="63"/>
       <c r="P32" s="64"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="60">
         <v>-549.04095472233598</v>
       </c>
@@ -9050,7 +9050,7 @@
       <c r="O33" s="63"/>
       <c r="P33" s="64"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="60">
         <v>-587.30895533624698</v>
       </c>
@@ -9093,7 +9093,7 @@
       <c r="O34" s="63"/>
       <c r="P34" s="64"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="60">
         <v>-625.57511687924398</v>
       </c>
@@ -9136,7 +9136,7 @@
       <c r="O35" s="63"/>
       <c r="P35" s="64"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="60">
         <v>-663.84066539860203</v>
       </c>
@@ -9179,7 +9179,7 @@
       <c r="O36" s="63"/>
       <c r="P36" s="64"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="60">
         <v>-702.104987870684</v>
       </c>
@@ -9222,7 +9222,7 @@
       <c r="O37" s="63"/>
       <c r="P37" s="64"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="60">
         <v>-740.36747127185197</v>
       </c>
@@ -9265,7 +9265,7 @@
       <c r="O38" s="63"/>
       <c r="P38" s="64"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="60">
         <v>-778.62934164938099</v>
       </c>
@@ -9308,7 +9308,7 @@
       <c r="O39" s="63"/>
       <c r="P39" s="64"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="60">
         <v>-816.88814690872005</v>
       </c>
@@ -9351,7 +9351,7 @@
       <c r="O40" s="63"/>
       <c r="P40" s="64"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="60">
         <v>-855.14633914442004</v>
       </c>
@@ -9394,7 +9394,7 @@
       <c r="O41" s="63"/>
       <c r="P41" s="64"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="60">
         <v>-893.40453138012003</v>
       </c>
@@ -9437,7 +9437,7 @@
       <c r="O42" s="63"/>
       <c r="P42" s="64"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="60">
         <v>-931.65781942671504</v>
       </c>
@@ -9480,7 +9480,7 @@
       <c r="O43" s="63"/>
       <c r="P43" s="64"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="60">
         <v>-969.90988142603396</v>
       </c>
@@ -9523,7 +9523,7 @@
       <c r="O44" s="63"/>
       <c r="P44" s="64"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="60">
         <v>-1008.15397411805</v>
       </c>
@@ -9566,7 +9566,7 @@
       <c r="O45" s="63"/>
       <c r="P45" s="64"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="60">
         <v>-1046.3962277391599</v>
       </c>
@@ -9609,7 +9609,7 @@
       <c r="O46" s="63"/>
       <c r="P46" s="64"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="60">
         <v>-1084.6305120529701</v>
       </c>
@@ -9652,7 +9652,7 @@
       <c r="O47" s="63"/>
       <c r="P47" s="64"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="60">
         <v>-1122.8660224140599</v>
       </c>
@@ -9682,7 +9682,7 @@
       <c r="O48" s="63"/>
       <c r="P48" s="64"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="60">
         <v>-1161.08743323147</v>
       </c>
@@ -9712,7 +9712,7 @@
       <c r="O49" s="63"/>
       <c r="P49" s="64"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="60">
         <v>-1199.30516590705</v>
       </c>
@@ -9742,7 +9742,7 @@
       <c r="O50" s="63"/>
       <c r="P50" s="64"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="60">
         <v>-1237.5192204407999</v>
       </c>
@@ -9772,7 +9772,7 @@
       <c r="O51" s="63"/>
       <c r="P51" s="64"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="60">
         <v>-1275.72530566725</v>
       </c>
@@ -9802,7 +9802,7 @@
       <c r="O52" s="63"/>
       <c r="P52" s="64"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="60">
         <v>-1313.9283257755101</v>
       </c>
@@ -9832,7 +9832,7 @@
       <c r="O53" s="63"/>
       <c r="P53" s="64"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="60">
         <v>-1352.1258286710299</v>
       </c>
@@ -9862,7 +9862,7 @@
       <c r="O54" s="63"/>
       <c r="P54" s="64"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="60">
         <v>-1390.3306878502101</v>
       </c>
@@ -9892,7 +9892,7 @@
       <c r="O55" s="63"/>
       <c r="P55" s="64"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="60">
         <v>-1428.5300298166501</v>
       </c>
@@ -9922,7 +9922,7 @@
       <c r="O56" s="63"/>
       <c r="P56" s="64"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="60">
         <v>-1466.7189503812299</v>
       </c>
@@ -9952,7 +9952,7 @@
       <c r="O57" s="63"/>
       <c r="P57" s="64"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="60">
         <v>-1499.6968635093899</v>
       </c>
@@ -9982,7 +9982,7 @@
       <c r="O58" s="63"/>
       <c r="P58" s="64"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J62" s="68"/>
       <c r="K62" s="51"/>
       <c r="L62" s="51"/>
@@ -9991,7 +9991,7 @@
       <c r="O62" s="51"/>
       <c r="P62" s="51"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H63" s="75" t="s">
         <v>198</v>
       </c>
@@ -10004,7 +10004,7 @@
       <c r="O63" s="51"/>
       <c r="P63" s="51"/>
     </row>
-    <row r="64" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" ht="15.6" x14ac:dyDescent="0.35">
       <c r="H64" s="69" t="s">
         <v>210</v>
       </c>
@@ -10019,7 +10019,7 @@
       <c r="O64" s="51"/>
       <c r="P64" s="51"/>
     </row>
-    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H65" s="70">
         <v>2.2997934048565084E-2</v>
       </c>
@@ -10035,7 +10035,7 @@
       <c r="O65" s="51"/>
       <c r="P65" s="51"/>
     </row>
-    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H66" s="70">
         <v>4.0069676396611777E-2</v>
       </c>
@@ -10051,7 +10051,7 @@
       <c r="O66" s="51"/>
       <c r="P66" s="51"/>
     </row>
-    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H67" s="70">
         <v>5.7084370034302737E-2</v>
       </c>
@@ -10067,7 +10067,7 @@
       <c r="O67" s="51"/>
       <c r="P67" s="51"/>
     </row>
-    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H68" s="70">
         <v>7.4140086301005395E-2</v>
       </c>
@@ -10083,7 +10083,7 @@
       <c r="O68" s="51"/>
       <c r="P68" s="51"/>
     </row>
-    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H69" s="70">
         <v>9.1140638350711872E-2</v>
       </c>
@@ -10099,7 +10099,7 @@
       <c r="O69" s="51"/>
       <c r="P69" s="51"/>
     </row>
-    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H70" s="70">
         <v>0.1080445517892699</v>
       </c>
@@ -10115,7 +10115,7 @@
       <c r="O70" s="51"/>
       <c r="P70" s="51"/>
     </row>
-    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H71" s="70">
         <v>0.12497606826753388</v>
       </c>
@@ -10131,7 +10131,7 @@
       <c r="O71" s="51"/>
       <c r="P71" s="51"/>
     </row>
-    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H72" s="70">
         <v>0.14198052165390951</v>
       </c>
@@ -10147,7 +10147,7 @@
       <c r="O72" s="51"/>
       <c r="P72" s="51"/>
     </row>
-    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H73" s="70">
         <v>0.15874470475517963</v>
       </c>
@@ -10163,7 +10163,7 @@
       <c r="O73" s="51"/>
       <c r="P73" s="51"/>
     </row>
-    <row r="74" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H74" s="70">
         <v>0.17553747925232432</v>
       </c>
@@ -10179,7 +10179,7 @@
       <c r="O74" s="51"/>
       <c r="P74" s="51"/>
     </row>
-    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H75" s="70">
         <v>0.19240417629290971</v>
       </c>
@@ -10195,7 +10195,7 @@
       <c r="O75" s="51"/>
       <c r="P75" s="51"/>
     </row>
-    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H76" s="70">
         <v>0.20901220546271423</v>
       </c>
@@ -10211,7 +10211,7 @@
       <c r="O76" s="51"/>
       <c r="P76" s="51"/>
     </row>
-    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H77" s="70">
         <v>0.22582431925537669</v>
       </c>
@@ -10227,7 +10227,7 @@
       <c r="O77" s="51"/>
       <c r="P77" s="51"/>
     </row>
-    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H78" s="70">
         <v>0.24236713011424937</v>
       </c>
@@ -10243,7 +10243,7 @@
       <c r="O78" s="51"/>
       <c r="P78" s="51"/>
     </row>
-    <row r="79" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H79" s="70">
         <v>0.25891734586657894</v>
       </c>
@@ -10259,7 +10259,7 @@
       <c r="O79" s="51"/>
       <c r="P79" s="51"/>
     </row>
-    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H80" s="70">
         <v>0.27532743679881172</v>
       </c>
@@ -10275,7 +10275,7 @@
       <c r="O80" s="51"/>
       <c r="P80" s="51"/>
     </row>
-    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H81" s="70">
         <v>0.29164753874763422</v>
       </c>
@@ -10291,7 +10291,7 @@
       <c r="O81" s="51"/>
       <c r="P81" s="51"/>
     </row>
-    <row r="82" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H82" s="70">
         <v>0.30783618288424536</v>
       </c>
@@ -10307,7 +10307,7 @@
       <c r="O82" s="51"/>
       <c r="P82" s="51"/>
     </row>
-    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H83" s="70">
         <v>0.32384418347196781</v>
       </c>
@@ -10323,7 +10323,7 @@
       <c r="O83" s="51"/>
       <c r="P83" s="51"/>
     </row>
-    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H84" s="70">
         <v>0.33973325501759533</v>
       </c>
@@ -10339,7 +10339,7 @@
       <c r="O84" s="51"/>
       <c r="P84" s="51"/>
     </row>
-    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H85" s="70">
         <v>0.3553317399203158</v>
       </c>
@@ -10355,7 +10355,7 @@
       <c r="O85" s="51"/>
       <c r="P85" s="51"/>
     </row>
-    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H86" s="70">
         <v>0.37078429028268828</v>
       </c>
@@ -10371,7 +10371,7 @@
       <c r="O86" s="51"/>
       <c r="P86" s="51"/>
     </row>
-    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H87" s="70">
         <v>0.38613044476352726</v>
       </c>
@@ -10387,7 +10387,7 @@
       <c r="O87" s="51"/>
       <c r="P87" s="51"/>
     </row>
-    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H88" s="70">
         <v>0.4009921758963842</v>
       </c>
@@ -10403,7 +10403,7 @@
       <c r="O88" s="51"/>
       <c r="P88" s="51"/>
     </row>
-    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H89" s="70">
         <v>0.4156182923872962</v>
       </c>
@@ -10419,7 +10419,7 @@
       <c r="O89" s="51"/>
       <c r="P89" s="51"/>
     </row>
-    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H90" s="70">
         <v>0.42943502667027428</v>
       </c>
@@ -10435,7 +10435,7 @@
       <c r="O90" s="51"/>
       <c r="P90" s="51"/>
     </row>
-    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H91" s="70">
         <v>0.44289756776749095</v>
       </c>
@@ -10451,7 +10451,7 @@
       <c r="O91" s="51"/>
       <c r="P91" s="51"/>
     </row>
-    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H92" s="70">
         <v>0.45543894715911687</v>
       </c>
@@ -10467,7 +10467,7 @@
       <c r="O92" s="51"/>
       <c r="P92" s="51"/>
     </row>
-    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H93" s="70">
         <v>0.46783735943015631</v>
       </c>
@@ -10483,7 +10483,7 @@
       <c r="O93" s="51"/>
       <c r="P93" s="51"/>
     </row>
-    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H94" s="70">
         <v>0.47863400366300879</v>
       </c>
@@ -10499,7 +10499,7 @@
       <c r="O94" s="51"/>
       <c r="P94" s="51"/>
     </row>
-    <row r="95" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H95" s="70">
         <v>0.48872859410433517</v>
       </c>
@@ -10515,7 +10515,7 @@
       <c r="O95" s="51"/>
       <c r="P95" s="51"/>
     </row>
-    <row r="96" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H96" s="70">
         <v>0.49808648675762501</v>
       </c>
@@ -10531,7 +10531,7 @@
       <c r="O96" s="51"/>
       <c r="P96" s="51"/>
     </row>
-    <row r="97" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H97" s="70">
         <v>0.50622094031681064</v>
       </c>
@@ -10547,7 +10547,7 @@
       <c r="O97" s="51"/>
       <c r="P97" s="51"/>
     </row>
-    <row r="98" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H98" s="70">
         <v>0.51358901063162188</v>
       </c>
@@ -10563,7 +10563,7 @@
       <c r="O98" s="51"/>
       <c r="P98" s="51"/>
     </row>
-    <row r="99" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H99" s="70">
         <v>0.51988812196851808</v>
       </c>
@@ -10579,7 +10579,7 @@
       <c r="O99" s="51"/>
       <c r="P99" s="51"/>
     </row>
-    <row r="100" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H100" s="70">
         <v>0.52654380991188665</v>
       </c>
@@ -10595,7 +10595,7 @@
       <c r="O100" s="51"/>
       <c r="P100" s="51"/>
     </row>
-    <row r="101" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H101" s="70">
         <v>0.53210746291493216</v>
       </c>
@@ -10611,7 +10611,7 @@
       <c r="O101" s="51"/>
       <c r="P101" s="51"/>
     </row>
-    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H102" s="70">
         <v>0.53593356457098895</v>
       </c>
@@ -10627,7 +10627,7 @@
       <c r="O102" s="51"/>
       <c r="P102" s="51"/>
     </row>
-    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:16" x14ac:dyDescent="0.3">
       <c r="H103" s="70">
         <v>0.53837802652041589</v>
       </c>
@@ -10643,7 +10643,7 @@
       <c r="O103" s="51"/>
       <c r="P103" s="51"/>
     </row>
-    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:16" x14ac:dyDescent="0.3">
       <c r="K104" s="51"/>
       <c r="L104" s="51"/>
       <c r="M104" s="51"/>

</xml_diff>